<commit_message>
init ayarları ekranda gösterme ok.
</commit_message>
<xml_diff>
--- a/7_Segment_Character.xlsx
+++ b/7_Segment_Character.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Saat_Termometre_DHT22.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24EEA061-6B1D-4B6A-AF6C-9E7928314153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C264D5-23DC-4C60-843D-4FF98BA3310B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E67F744A-9665-4DC9-B9C7-E5FA2EDD65C2}"/>
   </bookViews>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403186FE-D706-43B9-A319-73A7452E1641}">
-  <dimension ref="D6:X7"/>
+  <dimension ref="D6:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="M11" sqref="M11:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,6 +545,318 @@
         <v>B3</v>
       </c>
     </row>
+    <row r="8" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="str">
+        <f>DEC2HEX(K8*1+J8*2+I8*4+H8*8+G8*16+F8*32+E8*64+D8*128)</f>
+        <v>77</v>
+      </c>
+      <c r="O8">
+        <f>G8</f>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <f>H8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f>I8</f>
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <f>J8</f>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f>K8</f>
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f>D8</f>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f>F8</f>
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <f>E8</f>
+        <v>1</v>
+      </c>
+      <c r="X8" t="str">
+        <f>DEC2HEX(V8*1+U8*2+T8*4+S8*8+R8*16+Q8*32+P8*64+O8*128)</f>
+        <v>BB</v>
+      </c>
+    </row>
+    <row r="9" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ref="M9:M19" si="0">DEC2HEX(K9*1+J9*2+I9*4+H9*8+G9*16+F9*32+E9*64+D9*128)</f>
+        <v>7C</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:O11" si="1">G9</f>
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P11" si="2">H9</f>
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9:Q11" si="3">I9</f>
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ref="R9:R11" si="4">J9</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S9:S11" si="5">K9</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:T11" si="6">D9</f>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f t="shared" ref="U9:U11" si="7">F9</f>
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ref="V9:V11" si="8">E9</f>
+        <v>1</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" ref="X9:X11" si="9">DEC2HEX(V9*1+U9*2+T9*4+S9*8+R9*16+Q9*32+P9*64+O9*128)</f>
+        <v>E3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>5E</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="9"/>
+        <v>F1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="9"/>
+        <v>CB</v>
+      </c>
+    </row>
+    <row r="12" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:24" x14ac:dyDescent="0.25">
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>